<commit_message>
Dehalogenation data + PDF files of AFvsCS
</commit_message>
<xml_diff>
--- a/Dehalogenation_colorimetric_assays/Fluoride_concentrations+normalized_activities.xlsx
+++ b/Dehalogenation_colorimetric_assays/Fluoride_concentrations+normalized_activities.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Fluoride concentration" sheetId="2" r:id="rId1"/>
-    <sheet name="Data normalized Defluorination" sheetId="3" r:id="rId2"/>
+    <sheet name="Protein conc normalized defluo" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Data Fluoride concentration'!$C$106:$C$126</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="49">
   <si>
     <t>E</t>
   </si>
@@ -202,19 +202,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Pooled Standard deviation </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>in fraction of normalized WT activity</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Fluoride concentration / protein concentration in supernatant [</t>
     </r>
     <r>
@@ -253,6 +240,25 @@
   <si>
     <t>Defluorination activity normalized to WT activity</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pooled Standard deviation </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>[µM*mg^(-1)*ml]</t>
+    </r>
+  </si>
+  <si>
+    <t>SD pooled​=((Sum of Weighted Variances)/(​Sum of Degrees of Freedom))^0.5</t>
+  </si>
+  <si>
+    <t>Mean SD [µM*mg^(-1)*ml]</t>
+  </si>
 </sst>
 </file>
 
@@ -261,7 +267,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000000000000"/>
-    <numFmt numFmtId="174" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -274,6 +280,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -330,7 +337,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
@@ -339,11 +346,13 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,27 +361,7 @@
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1392,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BH126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9834,12 +9823,12 @@
         <v>10.348657964573258</v>
       </c>
       <c r="U103" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="104" spans="2:60" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="105" spans="2:60" x14ac:dyDescent="0.25">
@@ -10892,7 +10881,7 @@
         <v>1</v>
       </c>
       <c r="C125" s="12">
-        <f t="shared" ref="C125:N125" si="59">C99/$C$100</f>
+        <f t="shared" ref="C125:J125" si="59">C99/$C$100</f>
         <v>0.88826034955468769</v>
       </c>
       <c r="D125" s="12">
@@ -10933,7 +10922,7 @@
         <v>0</v>
       </c>
       <c r="C126" s="12">
-        <f t="shared" ref="C126:N126" si="60">C100/$C$100</f>
+        <f t="shared" ref="C126:H126" si="60">C100/$C$100</f>
         <v>1</v>
       </c>
       <c r="D126" s="12">
@@ -11010,8 +10999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BA206"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="A184" sqref="A184"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="L203" sqref="L203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18795,7 +18784,7 @@
     </row>
     <row r="76" spans="3:40" x14ac:dyDescent="0.35">
       <c r="C76">
-        <f t="shared" ref="C76:AN76" si="19">IF(C24&lt;100,C24,C50)</f>
+        <f t="shared" ref="C76:AJ76" si="19">IF(C24&lt;100,C24,C50)</f>
         <v>94.737737055983501</v>
       </c>
       <c r="D76">
@@ -18893,7 +18882,7 @@
     </row>
     <row r="77" spans="3:40" x14ac:dyDescent="0.35">
       <c r="C77">
-        <f t="shared" ref="C77:AN77" si="20">IF(C25&lt;100,C25,C51)</f>
+        <f t="shared" ref="C77:AH77" si="20">IF(C25&lt;100,C25,C51)</f>
         <v>111.85850317409447</v>
       </c>
       <c r="D77">
@@ -21405,7 +21394,7 @@
     </row>
     <row r="109" spans="2:40" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="111" spans="2:40" x14ac:dyDescent="0.35">
@@ -24184,7 +24173,7 @@
     </row>
     <row r="130" spans="2:53" x14ac:dyDescent="0.35">
       <c r="C130">
-        <f t="shared" ref="C130:AN130" si="40">C76/C103</f>
+        <f t="shared" ref="C130:AJ130" si="40">C76/C103</f>
         <v>1035.1588402096099</v>
       </c>
       <c r="D130">
@@ -24282,7 +24271,7 @@
     </row>
     <row r="131" spans="2:53" x14ac:dyDescent="0.35">
       <c r="C131">
-        <f t="shared" ref="C131:AN131" si="41">C77/C104</f>
+        <f t="shared" ref="C131:AH131" si="41">C77/C104</f>
         <v>869.5468219379236</v>
       </c>
       <c r="D131">
@@ -24356,10 +24345,10 @@
     </row>
     <row r="134" spans="2:53" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
+        <v>41</v>
+      </c>
+      <c r="P134" t="s">
         <v>42</v>
-      </c>
-      <c r="P134" t="s">
-        <v>43</v>
       </c>
       <c r="AC134" t="s">
         <v>38</v>
@@ -24518,51 +24507,51 @@
       <c r="B136" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C136">
+      <c r="C136" s="13">
         <f>AVERAGE(C111,P111,AC111)</f>
         <v>407.49035923456813</v>
       </c>
-      <c r="D136">
+      <c r="D136" s="13">
         <f t="shared" ref="D136:N136" si="42">AVERAGE(D111,Q111,AD111)</f>
         <v>192.08164525935345</v>
       </c>
-      <c r="E136">
+      <c r="E136" s="13">
         <f t="shared" si="42"/>
         <v>823.4473392308463</v>
       </c>
-      <c r="F136">
+      <c r="F136" s="13">
         <f t="shared" si="42"/>
         <v>435.40834566165069</v>
       </c>
-      <c r="G136">
+      <c r="G136" s="13">
         <f t="shared" si="42"/>
         <v>140.04936346917691</v>
       </c>
-      <c r="H136">
+      <c r="H136" s="13">
         <f t="shared" si="42"/>
         <v>276.36871276417827</v>
       </c>
-      <c r="I136">
+      <c r="I136" s="13">
         <f t="shared" si="42"/>
         <v>142.78801455938421</v>
       </c>
-      <c r="J136">
+      <c r="J136" s="13">
         <f t="shared" si="42"/>
         <v>68.340988760392335</v>
       </c>
-      <c r="K136">
+      <c r="K136" s="13">
         <f t="shared" si="42"/>
         <v>299.29965569391658</v>
       </c>
-      <c r="L136">
+      <c r="L136" s="13">
         <f t="shared" si="42"/>
         <v>52.506719995934013</v>
       </c>
-      <c r="M136">
+      <c r="M136" s="13">
         <f t="shared" si="42"/>
         <v>101.63477678958226</v>
       </c>
-      <c r="N136">
+      <c r="N136" s="13">
         <f t="shared" si="42"/>
         <v>855.82931442909319</v>
       </c>
@@ -24715,52 +24704,52 @@
       <c r="B137" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C137">
-        <f t="shared" ref="C137:C166" si="45">AVERAGE(C112,P112,AC112)</f>
+      <c r="C137" s="13">
+        <f t="shared" ref="C137:C156" si="45">AVERAGE(C112,P112,AC112)</f>
         <v>41.064222030792074</v>
       </c>
-      <c r="D137">
-        <f t="shared" ref="D137:D166" si="46">AVERAGE(D112,Q112,AD112)</f>
+      <c r="D137" s="13">
+        <f t="shared" ref="D137:D156" si="46">AVERAGE(D112,Q112,AD112)</f>
         <v>44.667521037275691</v>
       </c>
-      <c r="E137">
-        <f t="shared" ref="E137:E166" si="47">AVERAGE(E112,R112,AE112)</f>
+      <c r="E137" s="13">
+        <f t="shared" ref="E137:E156" si="47">AVERAGE(E112,R112,AE112)</f>
         <v>47.05273465324148</v>
       </c>
-      <c r="F137">
-        <f t="shared" ref="F137:F166" si="48">AVERAGE(F112,S112,AF112)</f>
+      <c r="F137" s="13">
+        <f t="shared" ref="F137:F156" si="48">AVERAGE(F112,S112,AF112)</f>
         <v>224.17290335071672</v>
       </c>
-      <c r="G137">
-        <f t="shared" ref="G137:G166" si="49">AVERAGE(G112,T112,AG112)</f>
+      <c r="G137" s="13">
+        <f t="shared" ref="G137:G156" si="49">AVERAGE(G112,T112,AG112)</f>
         <v>994.5980821974108</v>
       </c>
-      <c r="H137">
-        <f t="shared" ref="H137:H166" si="50">AVERAGE(H112,U112,AH112)</f>
+      <c r="H137" s="13">
+        <f t="shared" ref="H137:H156" si="50">AVERAGE(H112,U112,AH112)</f>
         <v>55.569231615508492</v>
       </c>
-      <c r="I137">
-        <f t="shared" ref="I137:I166" si="51">AVERAGE(I112,V112,AI112)</f>
+      <c r="I137" s="13">
+        <f t="shared" ref="I137:I155" si="51">AVERAGE(I112,V112,AI112)</f>
         <v>42.11978074719034</v>
       </c>
-      <c r="J137">
-        <f t="shared" ref="J137:J166" si="52">AVERAGE(J112,W112,AJ112)</f>
+      <c r="J137" s="13">
+        <f t="shared" ref="J137:J155" si="52">AVERAGE(J112,W112,AJ112)</f>
         <v>40.129583777577416</v>
       </c>
-      <c r="K137">
-        <f t="shared" ref="K137:K166" si="53">AVERAGE(K112,X112,AK112)</f>
+      <c r="K137" s="13">
+        <f t="shared" ref="K137:K154" si="53">AVERAGE(K112,X112,AK112)</f>
         <v>899.76515648343332</v>
       </c>
-      <c r="L137">
-        <f t="shared" ref="L137:L166" si="54">AVERAGE(L112,Y112,AL112)</f>
+      <c r="L137" s="13">
+        <f t="shared" ref="L137:L154" si="54">AVERAGE(L112,Y112,AL112)</f>
         <v>2544.129173032803</v>
       </c>
-      <c r="M137">
-        <f t="shared" ref="M137:M166" si="55">AVERAGE(M112,Z112,AM112)</f>
+      <c r="M137" s="13">
+        <f t="shared" ref="M137:M154" si="55">AVERAGE(M112,Z112,AM112)</f>
         <v>556.88384147530462</v>
       </c>
-      <c r="N137">
-        <f t="shared" ref="N137:N166" si="56">AVERAGE(N112,AA112,AN112)</f>
+      <c r="N137" s="13">
+        <f t="shared" ref="N137:N154" si="56">AVERAGE(N112,AA112,AN112)</f>
         <v>466.51482524974381</v>
       </c>
       <c r="P137">
@@ -24788,27 +24777,27 @@
         <v>6.1705729716111453</v>
       </c>
       <c r="V137">
-        <f t="shared" ref="V137:V156" si="63">_xlfn.STDEV.S(I112,V112,AI112)</f>
+        <f t="shared" ref="V137:V155" si="63">_xlfn.STDEV.S(I112,V112,AI112)</f>
         <v>10.153073071205664</v>
       </c>
       <c r="W137">
-        <f t="shared" ref="W137:W156" si="64">_xlfn.STDEV.S(J112,W112,AJ112)</f>
+        <f t="shared" ref="W137:W155" si="64">_xlfn.STDEV.S(J112,W112,AJ112)</f>
         <v>6.4607785609742612</v>
       </c>
       <c r="X137">
-        <f t="shared" ref="X137:X156" si="65">_xlfn.STDEV.S(K112,X112,AK112)</f>
+        <f t="shared" ref="X137:X154" si="65">_xlfn.STDEV.S(K112,X112,AK112)</f>
         <v>200.1208386539378</v>
       </c>
       <c r="Y137">
-        <f t="shared" ref="Y137:Y156" si="66">_xlfn.STDEV.S(L112,Y112,AL112)</f>
+        <f t="shared" ref="Y137:Y154" si="66">_xlfn.STDEV.S(L112,Y112,AL112)</f>
         <v>664.70951493548989</v>
       </c>
       <c r="Z137">
-        <f t="shared" ref="Z137:Z156" si="67">_xlfn.STDEV.S(M112,Z112,AM112)</f>
+        <f t="shared" ref="Z137:Z154" si="67">_xlfn.STDEV.S(M112,Z112,AM112)</f>
         <v>85.499022271720662</v>
       </c>
       <c r="AA137">
-        <f t="shared" ref="AA137:AA156" si="68">_xlfn.STDEV.S(N112,AA112,AN112)</f>
+        <f t="shared" ref="AA137:AA154" si="68">_xlfn.STDEV.S(N112,AA112,AN112)</f>
         <v>76.200203624646036</v>
       </c>
       <c r="AC137">
@@ -24836,27 +24825,27 @@
         <v>76.151941595956004</v>
       </c>
       <c r="AI137">
-        <f t="shared" ref="AI137:AI156" si="75">(V137^2)*2</f>
+        <f t="shared" ref="AI137:AI155" si="75">(V137^2)*2</f>
         <v>206.16978557848324</v>
       </c>
       <c r="AJ137">
-        <f t="shared" ref="AJ137:AJ156" si="76">(W137^2)*2</f>
+        <f t="shared" ref="AJ137:AJ155" si="76">(W137^2)*2</f>
         <v>83.483319227889297</v>
       </c>
       <c r="AK137">
-        <f t="shared" ref="AK137:AK156" si="77">(X137^2)*2</f>
+        <f t="shared" ref="AK137:AK154" si="77">(X137^2)*2</f>
         <v>80096.700127110802</v>
       </c>
       <c r="AL137">
-        <f t="shared" ref="AL137:AL156" si="78">(Y137^2)*2</f>
+        <f t="shared" ref="AL137:AL154" si="78">(Y137^2)*2</f>
         <v>883677.47849154857</v>
       </c>
       <c r="AM137">
-        <f t="shared" ref="AM137:AM156" si="79">(Z137^2)*2</f>
+        <f t="shared" ref="AM137:AM154" si="79">(Z137^2)*2</f>
         <v>14620.165618840372</v>
       </c>
       <c r="AN137">
-        <f t="shared" ref="AN137:AN156" si="80">(AA137^2)*2</f>
+        <f t="shared" ref="AN137:AN154" si="80">(AA137^2)*2</f>
         <v>11612.942064875038</v>
       </c>
       <c r="AP137">
@@ -24912,51 +24901,51 @@
       <c r="B138" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C138">
+      <c r="C138" s="13">
         <f t="shared" si="45"/>
         <v>960.87320496636676</v>
       </c>
-      <c r="D138">
+      <c r="D138" s="13">
         <f t="shared" si="46"/>
         <v>681.16430495962766</v>
       </c>
-      <c r="E138">
+      <c r="E138" s="13">
         <f t="shared" si="47"/>
         <v>150.68451788459137</v>
       </c>
-      <c r="F138">
+      <c r="F138" s="13">
         <f t="shared" si="48"/>
         <v>909.84299621081618</v>
       </c>
-      <c r="G138">
+      <c r="G138" s="13">
         <f t="shared" si="49"/>
         <v>463.66960083987215</v>
       </c>
-      <c r="H138">
+      <c r="H138" s="13">
         <f t="shared" si="50"/>
         <v>97.539679890686713</v>
       </c>
-      <c r="I138">
+      <c r="I138" s="13">
         <f t="shared" si="51"/>
         <v>898.45217700752471</v>
       </c>
-      <c r="J138">
+      <c r="J138" s="13">
         <f t="shared" si="52"/>
         <v>1053.6573335594626</v>
       </c>
-      <c r="K138">
+      <c r="K138" s="13">
         <f t="shared" si="53"/>
         <v>901.25133088676228</v>
       </c>
-      <c r="L138">
+      <c r="L138" s="13">
         <f t="shared" si="54"/>
         <v>878.59557263782187</v>
       </c>
-      <c r="M138">
+      <c r="M138" s="13">
         <f t="shared" si="55"/>
         <v>994.08819623073589</v>
       </c>
-      <c r="N138">
+      <c r="N138" s="13">
         <f t="shared" si="56"/>
         <v>698.15261040884161</v>
       </c>
@@ -25109,51 +25098,51 @@
       <c r="B139" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C139">
+      <c r="C139" s="13">
         <f t="shared" si="45"/>
         <v>626.43074096949272</v>
       </c>
-      <c r="D139">
+      <c r="D139" s="13">
         <f t="shared" si="46"/>
         <v>263.71482532579989</v>
       </c>
-      <c r="E139">
+      <c r="E139" s="13">
         <f t="shared" si="47"/>
         <v>396.71845280267854</v>
       </c>
-      <c r="F139">
+      <c r="F139" s="13">
         <f t="shared" si="48"/>
         <v>46.151688540074325</v>
       </c>
-      <c r="G139">
+      <c r="G139" s="13">
         <f t="shared" si="49"/>
         <v>874.4541995444265</v>
       </c>
-      <c r="H139">
+      <c r="H139" s="13">
         <f t="shared" si="50"/>
         <v>740.09337498378409</v>
       </c>
-      <c r="I139">
+      <c r="I139" s="13">
         <f t="shared" si="51"/>
         <v>45.236554058736964</v>
       </c>
-      <c r="J139">
+      <c r="J139" s="13">
         <f t="shared" si="52"/>
         <v>41.032620730181783</v>
       </c>
-      <c r="K139">
+      <c r="K139" s="13">
         <f t="shared" si="53"/>
         <v>413.72125151073442</v>
       </c>
-      <c r="L139">
+      <c r="L139" s="13">
         <f t="shared" si="54"/>
         <v>833.46746112658423</v>
       </c>
-      <c r="M139">
+      <c r="M139" s="13">
         <f t="shared" si="55"/>
         <v>50.885843097902011</v>
       </c>
-      <c r="N139">
+      <c r="N139" s="13">
         <f t="shared" si="56"/>
         <v>49.678151988092772</v>
       </c>
@@ -25306,51 +25295,51 @@
       <c r="B140" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C140">
+      <c r="C140" s="13">
         <f t="shared" si="45"/>
         <v>859.12288415680553</v>
       </c>
-      <c r="D140">
+      <c r="D140" s="13">
         <f t="shared" si="46"/>
         <v>806.21355582486376</v>
       </c>
-      <c r="E140">
+      <c r="E140" s="13">
         <f t="shared" si="47"/>
         <v>1069.7808300686431</v>
       </c>
-      <c r="F140">
+      <c r="F140" s="13">
         <f t="shared" si="48"/>
         <v>144.21188113795878</v>
       </c>
-      <c r="G140">
+      <c r="G140" s="13">
         <f t="shared" si="49"/>
         <v>1048.5444416560561</v>
       </c>
-      <c r="H140">
+      <c r="H140" s="13">
         <f t="shared" si="50"/>
         <v>817.20341602239512</v>
       </c>
-      <c r="I140">
+      <c r="I140" s="13">
         <f t="shared" si="51"/>
         <v>173.49876252457429</v>
       </c>
-      <c r="J140">
+      <c r="J140" s="13">
         <f t="shared" si="52"/>
         <v>936.69303859261061</v>
       </c>
-      <c r="K140">
+      <c r="K140" s="13">
         <f t="shared" si="53"/>
         <v>523.39861405164584</v>
       </c>
-      <c r="L140">
+      <c r="L140" s="13">
         <f t="shared" si="54"/>
         <v>880.57086028823107</v>
       </c>
-      <c r="M140">
+      <c r="M140" s="13">
         <f t="shared" si="55"/>
         <v>403.12898554122256</v>
       </c>
-      <c r="N140">
+      <c r="N140" s="13">
         <f t="shared" si="56"/>
         <v>133.99350452510768</v>
       </c>
@@ -25503,51 +25492,51 @@
       <c r="B141" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C141">
+      <c r="C141" s="13">
         <f t="shared" si="45"/>
         <v>1654.8174901008208</v>
       </c>
-      <c r="D141">
+      <c r="D141" s="13">
         <f t="shared" si="46"/>
         <v>854.28536718946043</v>
       </c>
-      <c r="E141">
+      <c r="E141" s="13">
         <f t="shared" si="47"/>
         <v>1162.6719683932824</v>
       </c>
-      <c r="F141">
+      <c r="F141" s="13">
         <f t="shared" si="48"/>
         <v>1133.6498689181208</v>
       </c>
-      <c r="G141">
+      <c r="G141" s="13">
         <f t="shared" si="49"/>
         <v>1048.6590161837291</v>
       </c>
-      <c r="H141">
+      <c r="H141" s="13">
         <f t="shared" si="50"/>
         <v>51.999483142247151</v>
       </c>
-      <c r="I141">
+      <c r="I141" s="13">
         <f t="shared" si="51"/>
         <v>683.54803138850968</v>
       </c>
-      <c r="J141">
+      <c r="J141" s="13">
         <f t="shared" si="52"/>
         <v>1217.7661235473988</v>
       </c>
-      <c r="K141">
+      <c r="K141" s="13">
         <f t="shared" si="53"/>
         <v>48.841839198555782</v>
       </c>
-      <c r="L141">
+      <c r="L141" s="13">
         <f t="shared" si="54"/>
         <v>126.7069837496753</v>
       </c>
-      <c r="M141">
+      <c r="M141" s="13">
         <f t="shared" si="55"/>
         <v>57.833250344042504</v>
       </c>
-      <c r="N141">
+      <c r="N141" s="13">
         <f t="shared" si="56"/>
         <v>108.8011702830579</v>
       </c>
@@ -25700,51 +25689,51 @@
       <c r="B142" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C142">
+      <c r="C142" s="13">
         <f t="shared" si="45"/>
         <v>62.664309534506401</v>
       </c>
-      <c r="D142">
+      <c r="D142" s="13">
         <f t="shared" si="46"/>
         <v>287.55422846261291</v>
       </c>
-      <c r="E142">
+      <c r="E142" s="13">
         <f t="shared" si="47"/>
         <v>795.39840644296237</v>
       </c>
-      <c r="F142">
+      <c r="F142" s="13">
         <f t="shared" si="48"/>
         <v>404.75738192318613</v>
       </c>
-      <c r="G142">
+      <c r="G142" s="13">
         <f t="shared" si="49"/>
         <v>75.862338431742756</v>
       </c>
-      <c r="H142">
+      <c r="H142" s="13">
         <f t="shared" si="50"/>
         <v>1602.533553646557</v>
       </c>
-      <c r="I142">
+      <c r="I142" s="13">
         <f t="shared" si="51"/>
         <v>1391.1502462429542</v>
       </c>
-      <c r="J142">
+      <c r="J142" s="13">
         <f t="shared" si="52"/>
         <v>56.767478473878498</v>
       </c>
-      <c r="K142">
+      <c r="K142" s="13">
         <f t="shared" si="53"/>
         <v>821.47832156199036</v>
       </c>
-      <c r="L142">
+      <c r="L142" s="13">
         <f t="shared" si="54"/>
         <v>1210.2121784464273</v>
       </c>
-      <c r="M142">
+      <c r="M142" s="13">
         <f t="shared" si="55"/>
         <v>939.43910981004228</v>
       </c>
-      <c r="N142">
+      <c r="N142" s="13">
         <f t="shared" si="56"/>
         <v>716.35563954627469</v>
       </c>
@@ -25897,51 +25886,51 @@
       <c r="B143" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C143">
+      <c r="C143" s="13">
         <f t="shared" si="45"/>
         <v>1379.141916040586</v>
       </c>
-      <c r="D143">
+      <c r="D143" s="13">
         <f t="shared" si="46"/>
         <v>84.534425383051328</v>
       </c>
-      <c r="E143">
+      <c r="E143" s="13">
         <f t="shared" si="47"/>
         <v>991.06047895433983</v>
       </c>
-      <c r="F143">
+      <c r="F143" s="13">
         <f t="shared" si="48"/>
         <v>360.18361990767545</v>
       </c>
-      <c r="G143">
+      <c r="G143" s="13">
         <f t="shared" si="49"/>
         <v>1056.7592572170481</v>
       </c>
-      <c r="H143">
+      <c r="H143" s="13">
         <f t="shared" si="50"/>
         <v>1173.9543330753836</v>
       </c>
-      <c r="I143">
+      <c r="I143" s="13">
         <f t="shared" si="51"/>
         <v>1430.8967095730829</v>
       </c>
-      <c r="J143">
+      <c r="J143" s="13">
         <f t="shared" si="52"/>
         <v>236.91913031174042</v>
       </c>
-      <c r="K143">
+      <c r="K143" s="13">
         <f t="shared" si="53"/>
         <v>1383.7162087122967</v>
       </c>
-      <c r="L143">
+      <c r="L143" s="13">
         <f t="shared" si="54"/>
         <v>1543.8856078830916</v>
       </c>
-      <c r="M143">
+      <c r="M143" s="13">
         <f t="shared" si="55"/>
         <v>1086.8873619223366</v>
       </c>
-      <c r="N143">
+      <c r="N143" s="13">
         <f t="shared" si="56"/>
         <v>69.414842254962551</v>
       </c>
@@ -26094,51 +26083,51 @@
       <c r="B144" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C144">
+      <c r="C144" s="13">
         <f t="shared" si="45"/>
         <v>918.48958422916439</v>
       </c>
-      <c r="D144">
+      <c r="D144" s="13">
         <f t="shared" si="46"/>
         <v>912.94675500473716</v>
       </c>
-      <c r="E144">
+      <c r="E144" s="13">
         <f t="shared" si="47"/>
         <v>888.18108251646083</v>
       </c>
-      <c r="F144">
+      <c r="F144" s="13">
         <f t="shared" si="48"/>
         <v>49.201493579388206</v>
       </c>
-      <c r="G144">
+      <c r="G144" s="13">
         <f t="shared" si="49"/>
         <v>72.531014913590028</v>
       </c>
-      <c r="H144">
+      <c r="H144" s="13">
         <f t="shared" si="50"/>
         <v>109.59352584695762</v>
       </c>
-      <c r="I144">
+      <c r="I144" s="13">
         <f t="shared" si="51"/>
         <v>737.40915680089017</v>
       </c>
-      <c r="J144">
+      <c r="J144" s="13">
         <f t="shared" si="52"/>
         <v>1452.3159624388693</v>
       </c>
-      <c r="K144">
+      <c r="K144" s="13">
         <f t="shared" si="53"/>
         <v>280.91946713521736</v>
       </c>
-      <c r="L144">
+      <c r="L144" s="13">
         <f t="shared" si="54"/>
         <v>34.942358723334898</v>
       </c>
-      <c r="M144">
+      <c r="M144" s="13">
         <f t="shared" si="55"/>
         <v>777.36766339499025</v>
       </c>
-      <c r="N144">
+      <c r="N144" s="13">
         <f t="shared" si="56"/>
         <v>43.051370449839048</v>
       </c>
@@ -26291,51 +26280,51 @@
       <c r="B145" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C145">
+      <c r="C145" s="13">
         <f t="shared" si="45"/>
         <v>1221.1612756225695</v>
       </c>
-      <c r="D145">
+      <c r="D145" s="13">
         <f t="shared" si="46"/>
         <v>1144.959186499276</v>
       </c>
-      <c r="E145">
+      <c r="E145" s="13">
         <f t="shared" si="47"/>
         <v>944.11113348683011</v>
       </c>
-      <c r="F145">
+      <c r="F145" s="13">
         <f t="shared" si="48"/>
         <v>1793.9671689112276</v>
       </c>
-      <c r="G145">
+      <c r="G145" s="13">
         <f t="shared" si="49"/>
         <v>47.60009691862539</v>
       </c>
-      <c r="H145">
+      <c r="H145" s="13">
         <f t="shared" si="50"/>
         <v>1403.8799927580224</v>
       </c>
-      <c r="I145">
+      <c r="I145" s="13">
         <f t="shared" si="51"/>
         <v>1154.6446623322402</v>
       </c>
-      <c r="J145">
+      <c r="J145" s="13">
         <f t="shared" si="52"/>
         <v>44.49619601567764</v>
       </c>
-      <c r="K145">
+      <c r="K145" s="13">
         <f t="shared" si="53"/>
         <v>890.72153933214361</v>
       </c>
-      <c r="L145">
+      <c r="L145" s="13">
         <f t="shared" si="54"/>
         <v>1034.6722885409417</v>
       </c>
-      <c r="M145">
+      <c r="M145" s="13">
         <f t="shared" si="55"/>
         <v>774.34744825152529</v>
       </c>
-      <c r="N145">
+      <c r="N145" s="13">
         <f t="shared" si="56"/>
         <v>39.665630328755093</v>
       </c>
@@ -26488,51 +26477,51 @@
       <c r="B146" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C146">
+      <c r="C146" s="13">
         <f t="shared" si="45"/>
         <v>2535.112088311786</v>
       </c>
-      <c r="D146">
+      <c r="D146" s="13">
         <f t="shared" si="46"/>
         <v>47.939194562922218</v>
       </c>
-      <c r="E146">
+      <c r="E146" s="13">
         <f t="shared" si="47"/>
         <v>248.46347082554561</v>
       </c>
-      <c r="F146">
+      <c r="F146" s="13">
         <f t="shared" si="48"/>
         <v>509.63536919318739</v>
       </c>
-      <c r="G146">
+      <c r="G146" s="13">
         <f t="shared" si="49"/>
         <v>48.254246868364788</v>
       </c>
-      <c r="H146">
+      <c r="H146" s="13">
         <f t="shared" si="50"/>
         <v>69.532901721885381</v>
       </c>
-      <c r="I146">
+      <c r="I146" s="13">
         <f t="shared" si="51"/>
         <v>48.986655595101126</v>
       </c>
-      <c r="J146">
+      <c r="J146" s="13">
         <f t="shared" si="52"/>
         <v>332.4490110476699</v>
       </c>
-      <c r="K146">
+      <c r="K146" s="13">
         <f t="shared" si="53"/>
         <v>46.533132957918582</v>
       </c>
-      <c r="L146">
+      <c r="L146" s="13">
         <f t="shared" si="54"/>
         <v>46.089335629177633</v>
       </c>
-      <c r="M146">
+      <c r="M146" s="13">
         <f t="shared" si="55"/>
         <v>159.22040999381917</v>
       </c>
-      <c r="N146">
+      <c r="N146" s="13">
         <f t="shared" si="56"/>
         <v>780.89600028795246</v>
       </c>
@@ -26685,51 +26674,51 @@
       <c r="B147" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C147">
+      <c r="C147" s="13">
         <f t="shared" si="45"/>
         <v>41.357007490033958</v>
       </c>
-      <c r="D147">
+      <c r="D147" s="13">
         <f t="shared" si="46"/>
         <v>98.153603605062514</v>
       </c>
-      <c r="E147">
+      <c r="E147" s="13">
         <f t="shared" si="47"/>
         <v>71.403408306266371</v>
       </c>
-      <c r="F147">
+      <c r="F147" s="13">
         <f t="shared" si="48"/>
         <v>46.213886420877692</v>
       </c>
-      <c r="G147">
+      <c r="G147" s="13">
         <f t="shared" si="49"/>
         <v>41.75456447107652</v>
       </c>
-      <c r="H147">
+      <c r="H147" s="13">
         <f t="shared" si="50"/>
         <v>359.04692497639218</v>
       </c>
-      <c r="I147">
+      <c r="I147" s="13">
         <f t="shared" si="51"/>
         <v>3119.4707950333436</v>
       </c>
-      <c r="J147">
+      <c r="J147" s="13">
         <f t="shared" si="52"/>
         <v>2192.7460981222075</v>
       </c>
-      <c r="K147">
+      <c r="K147" s="13">
         <f t="shared" si="53"/>
         <v>883.83518763638187</v>
       </c>
-      <c r="L147">
+      <c r="L147" s="13">
         <f t="shared" si="54"/>
         <v>39.870176721018538</v>
       </c>
-      <c r="M147">
+      <c r="M147" s="13">
         <f t="shared" si="55"/>
         <v>667.20764189072258</v>
       </c>
-      <c r="N147">
+      <c r="N147" s="13">
         <f t="shared" si="56"/>
         <v>42.389568394794019</v>
       </c>
@@ -26882,51 +26871,51 @@
       <c r="B148" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C148">
+      <c r="C148" s="13">
         <f t="shared" si="45"/>
         <v>58.179548747217474</v>
       </c>
-      <c r="D148">
+      <c r="D148" s="13">
         <f t="shared" si="46"/>
         <v>40.914484577829711</v>
       </c>
-      <c r="E148">
+      <c r="E148" s="13">
         <f t="shared" si="47"/>
         <v>39.362682652794781</v>
       </c>
-      <c r="F148">
+      <c r="F148" s="13">
         <f t="shared" si="48"/>
         <v>46.776085904799196</v>
       </c>
-      <c r="G148">
+      <c r="G148" s="13">
         <f t="shared" si="49"/>
         <v>45.947721782671131</v>
       </c>
-      <c r="H148">
+      <c r="H148" s="13">
         <f t="shared" si="50"/>
         <v>1549.8621028760599</v>
       </c>
-      <c r="I148">
+      <c r="I148" s="13">
         <f t="shared" si="51"/>
         <v>107.88799005739342</v>
       </c>
-      <c r="J148">
+      <c r="J148" s="13">
         <f t="shared" si="52"/>
         <v>644.99033125583128</v>
       </c>
-      <c r="K148">
+      <c r="K148" s="13">
         <f t="shared" si="53"/>
         <v>46.243359507966126</v>
       </c>
-      <c r="L148">
+      <c r="L148" s="13">
         <f t="shared" si="54"/>
         <v>644.96956663889148</v>
       </c>
-      <c r="M148">
+      <c r="M148" s="13">
         <f t="shared" si="55"/>
         <v>57.668495395118747</v>
       </c>
-      <c r="N148">
+      <c r="N148" s="13">
         <f t="shared" si="56"/>
         <v>153.34087604686161</v>
       </c>
@@ -27079,51 +27068,51 @@
       <c r="B149" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C149">
+      <c r="C149" s="13">
         <f t="shared" si="45"/>
         <v>45.083143441034053</v>
       </c>
-      <c r="D149">
+      <c r="D149" s="13">
         <f t="shared" si="46"/>
         <v>48.794102673204975</v>
       </c>
-      <c r="E149">
+      <c r="E149" s="13">
         <f t="shared" si="47"/>
         <v>273.32373249485954</v>
       </c>
-      <c r="F149">
+      <c r="F149" s="13">
         <f t="shared" si="48"/>
         <v>82.730522616526329</v>
       </c>
-      <c r="G149">
+      <c r="G149" s="13">
         <f t="shared" si="49"/>
         <v>436.14871044741312</v>
       </c>
-      <c r="H149">
+      <c r="H149" s="13">
         <f t="shared" si="50"/>
         <v>62.998579950022112</v>
       </c>
-      <c r="I149">
+      <c r="I149" s="13">
         <f t="shared" si="51"/>
         <v>40.322279541595428</v>
       </c>
-      <c r="J149">
+      <c r="J149" s="13">
         <f t="shared" si="52"/>
         <v>1323.884480240655</v>
       </c>
-      <c r="K149">
+      <c r="K149" s="13">
         <f t="shared" si="53"/>
         <v>894.16243200627559</v>
       </c>
-      <c r="L149">
+      <c r="L149" s="13">
         <f t="shared" si="54"/>
         <v>39.470138635567196</v>
       </c>
-      <c r="M149">
+      <c r="M149" s="13">
         <f t="shared" si="55"/>
         <v>53.608171337929015</v>
       </c>
-      <c r="N149">
+      <c r="N149" s="13">
         <f t="shared" si="56"/>
         <v>1633.6627819865835</v>
       </c>
@@ -27276,51 +27265,51 @@
       <c r="B150" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C150">
+      <c r="C150" s="13">
         <f t="shared" si="45"/>
         <v>48.45102044709413</v>
       </c>
-      <c r="D150">
+      <c r="D150" s="13">
         <f t="shared" si="46"/>
         <v>46.825454507164601</v>
       </c>
-      <c r="E150">
+      <c r="E150" s="13">
         <f t="shared" si="47"/>
         <v>42.319725618950692</v>
       </c>
-      <c r="F150">
+      <c r="F150" s="13">
         <f t="shared" si="48"/>
         <v>340.3502547787071</v>
       </c>
-      <c r="G150">
+      <c r="G150" s="13">
         <f t="shared" si="49"/>
         <v>1007.5569933262137</v>
       </c>
-      <c r="H150">
+      <c r="H150" s="13">
         <f t="shared" si="50"/>
         <v>1053.7436060962691</v>
       </c>
-      <c r="I150">
+      <c r="I150" s="13">
         <f t="shared" si="51"/>
         <v>808.94475565205857</v>
       </c>
-      <c r="J150">
+      <c r="J150" s="13">
         <f t="shared" si="52"/>
         <v>61.463325252796324</v>
       </c>
-      <c r="K150">
+      <c r="K150" s="13">
         <f t="shared" si="53"/>
         <v>50.986864617346946</v>
       </c>
-      <c r="L150">
+      <c r="L150" s="13">
         <f t="shared" si="54"/>
         <v>510.72048531466527</v>
       </c>
-      <c r="M150">
+      <c r="M150" s="13">
         <f t="shared" si="55"/>
         <v>46.719881385790295</v>
       </c>
-      <c r="N150">
+      <c r="N150" s="13">
         <f t="shared" si="56"/>
         <v>70.529708303371521</v>
       </c>
@@ -27473,51 +27462,51 @@
       <c r="B151" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C151">
+      <c r="C151" s="13">
         <f t="shared" si="45"/>
         <v>52.493075580822108</v>
       </c>
-      <c r="D151">
+      <c r="D151" s="13">
         <f t="shared" si="46"/>
         <v>61.779922876082878</v>
       </c>
-      <c r="E151">
+      <c r="E151" s="13">
         <f t="shared" si="47"/>
         <v>41.470169115153446</v>
       </c>
-      <c r="F151">
+      <c r="F151" s="13">
         <f t="shared" si="48"/>
         <v>924.58961053130827</v>
       </c>
-      <c r="G151">
+      <c r="G151" s="13">
         <f t="shared" si="49"/>
         <v>767.38326361605107</v>
       </c>
-      <c r="H151">
+      <c r="H151" s="13">
         <f t="shared" si="50"/>
         <v>33.114503584391066</v>
       </c>
-      <c r="I151">
+      <c r="I151" s="13">
         <f t="shared" si="51"/>
         <v>58.320568780023017</v>
       </c>
-      <c r="J151">
+      <c r="J151" s="13">
         <f t="shared" si="52"/>
         <v>47.38485283725803</v>
       </c>
-      <c r="K151">
+      <c r="K151" s="13">
         <f t="shared" si="53"/>
         <v>341.84418296598602</v>
       </c>
-      <c r="L151">
+      <c r="L151" s="13">
         <f t="shared" si="54"/>
         <v>52.576344091154709</v>
       </c>
-      <c r="M151">
+      <c r="M151" s="13">
         <f t="shared" si="55"/>
         <v>1644.6027397460275</v>
       </c>
-      <c r="N151">
+      <c r="N151" s="13">
         <f t="shared" si="56"/>
         <v>1134.6917273387401</v>
       </c>
@@ -27670,51 +27659,51 @@
       <c r="B152" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C152">
+      <c r="C152" s="13">
         <f t="shared" si="45"/>
         <v>159.39653058450256</v>
       </c>
-      <c r="D152">
+      <c r="D152" s="13">
         <f t="shared" si="46"/>
         <v>56.337629829247668</v>
       </c>
-      <c r="E152">
+      <c r="E152" s="13">
         <f t="shared" si="47"/>
         <v>134.16721332392331</v>
       </c>
-      <c r="F152">
+      <c r="F152" s="13">
         <f t="shared" si="48"/>
         <v>862.7469776658512</v>
       </c>
-      <c r="G152">
+      <c r="G152" s="13">
         <f t="shared" si="49"/>
         <v>57.222735016663513</v>
       </c>
-      <c r="H152">
+      <c r="H152" s="13">
         <f t="shared" si="50"/>
         <v>722.74056811763978</v>
       </c>
-      <c r="I152">
+      <c r="I152" s="13">
         <f t="shared" si="51"/>
         <v>508.12320467771048</v>
       </c>
-      <c r="J152">
+      <c r="J152" s="13">
         <f t="shared" si="52"/>
         <v>70.641006015865898</v>
       </c>
-      <c r="K152">
+      <c r="K152" s="13">
         <f t="shared" si="53"/>
         <v>214.0104447008562</v>
       </c>
-      <c r="L152">
+      <c r="L152" s="13">
         <f t="shared" si="54"/>
         <v>47.573853752079032</v>
       </c>
-      <c r="M152">
+      <c r="M152" s="13">
         <f t="shared" si="55"/>
         <v>684.99955521175013</v>
       </c>
-      <c r="N152">
+      <c r="N152" s="13">
         <f t="shared" si="56"/>
         <v>1104.0616533123716</v>
       </c>
@@ -27867,51 +27856,51 @@
       <c r="B153" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C153">
+      <c r="C153" s="13">
         <f t="shared" si="45"/>
         <v>48.662417407589601</v>
       </c>
-      <c r="D153">
+      <c r="D153" s="13">
         <f t="shared" si="46"/>
         <v>36.858325142493698</v>
       </c>
-      <c r="E153">
+      <c r="E153" s="13">
         <f t="shared" si="47"/>
         <v>60.824390712964288</v>
       </c>
-      <c r="F153">
+      <c r="F153" s="13">
         <f t="shared" si="48"/>
         <v>949.18973402171366</v>
       </c>
-      <c r="G153">
+      <c r="G153" s="13">
         <f t="shared" si="49"/>
         <v>1042.4557822055333</v>
       </c>
-      <c r="H153">
+      <c r="H153" s="13">
         <f t="shared" si="50"/>
         <v>863.27337523643826</v>
       </c>
-      <c r="I153">
+      <c r="I153" s="13">
         <f t="shared" si="51"/>
         <v>874.32943766120013</v>
       </c>
-      <c r="J153">
+      <c r="J153" s="13">
         <f t="shared" si="52"/>
         <v>115.40766887758656</v>
       </c>
-      <c r="K153">
+      <c r="K153" s="13">
         <f t="shared" si="53"/>
         <v>776.28106474778861</v>
       </c>
-      <c r="L153">
+      <c r="L153" s="13">
         <f t="shared" si="54"/>
         <v>231.92682931989995</v>
       </c>
-      <c r="M153">
+      <c r="M153" s="13">
         <f t="shared" si="55"/>
         <v>748.1023542734107</v>
       </c>
-      <c r="N153">
+      <c r="N153" s="13">
         <f t="shared" si="56"/>
         <v>1023.340124396345</v>
       </c>
@@ -28064,51 +28053,51 @@
       <c r="B154" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C154">
+      <c r="C154" s="13">
         <f t="shared" si="45"/>
         <v>626.63092684517039</v>
       </c>
-      <c r="D154">
+      <c r="D154" s="13">
         <f t="shared" si="46"/>
         <v>882.28373659871579</v>
       </c>
-      <c r="E154">
+      <c r="E154" s="13">
         <f t="shared" si="47"/>
         <v>137.83668273336502</v>
       </c>
-      <c r="F154">
+      <c r="F154" s="13">
         <f t="shared" si="48"/>
         <v>1097.6864576978558</v>
       </c>
-      <c r="G154">
+      <c r="G154" s="13">
         <f t="shared" si="49"/>
         <v>53.003074948386733</v>
       </c>
-      <c r="H154">
+      <c r="H154" s="13">
         <f t="shared" si="50"/>
         <v>819.82817409632423</v>
       </c>
-      <c r="I154">
+      <c r="I154" s="13">
         <f t="shared" si="51"/>
         <v>994.21398339623045</v>
       </c>
-      <c r="J154">
+      <c r="J154" s="13">
         <f t="shared" si="52"/>
         <v>554.85004877297717</v>
       </c>
-      <c r="K154">
+      <c r="K154" s="13">
         <f t="shared" si="53"/>
         <v>928.71431518442296</v>
       </c>
-      <c r="L154">
+      <c r="L154" s="13">
         <f t="shared" si="54"/>
         <v>35.382065579989408</v>
       </c>
-      <c r="M154">
+      <c r="M154" s="13">
         <f t="shared" si="55"/>
         <v>38.063106044208887</v>
       </c>
-      <c r="N154">
+      <c r="N154" s="13">
         <f t="shared" si="56"/>
         <v>812.66059543265158</v>
       </c>
@@ -28261,38 +28250,42 @@
       <c r="B155" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C155">
+      <c r="C155" s="13">
         <f t="shared" si="45"/>
         <v>1018.0045896872829</v>
       </c>
-      <c r="D155">
+      <c r="D155" s="13">
         <f t="shared" si="46"/>
         <v>56.825508729438475</v>
       </c>
-      <c r="E155">
+      <c r="E155" s="13">
         <f t="shared" si="47"/>
         <v>108.10901850353189</v>
       </c>
-      <c r="F155">
+      <c r="F155" s="13">
         <f t="shared" si="48"/>
         <v>1085.1082932694783</v>
       </c>
-      <c r="G155">
+      <c r="G155" s="13">
         <f t="shared" si="49"/>
         <v>1081.1684344743312</v>
       </c>
-      <c r="H155">
+      <c r="H155" s="13">
         <f t="shared" si="50"/>
         <v>63.855177181234119</v>
       </c>
-      <c r="I155">
+      <c r="I155" s="13">
         <f t="shared" si="51"/>
         <v>340.43823392808309</v>
       </c>
-      <c r="J155">
+      <c r="J155" s="13">
         <f t="shared" si="52"/>
         <v>1179.6195213044593</v>
       </c>
+      <c r="K155" s="13"/>
+      <c r="L155" s="13"/>
+      <c r="M155" s="13"/>
+      <c r="N155" s="13"/>
       <c r="P155">
         <f t="shared" si="57"/>
         <v>310.68863100381247</v>
@@ -28394,30 +28387,36 @@
       <c r="B156" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C156">
+      <c r="C156" s="13">
         <f t="shared" si="45"/>
         <v>830.71760292800764</v>
       </c>
-      <c r="D156">
+      <c r="D156" s="13">
         <f t="shared" si="46"/>
         <v>3070.3170161991911</v>
       </c>
-      <c r="E156">
+      <c r="E156" s="13">
         <f t="shared" si="47"/>
         <v>111.73101435381415</v>
       </c>
-      <c r="F156">
+      <c r="F156" s="13">
         <f t="shared" si="48"/>
         <v>103.72666975955275</v>
       </c>
-      <c r="G156">
+      <c r="G156" s="13">
         <f t="shared" si="49"/>
         <v>130.38718634946005</v>
       </c>
-      <c r="H156">
+      <c r="H156" s="13">
         <f t="shared" si="50"/>
         <v>25.975217448794339</v>
       </c>
+      <c r="I156" s="13"/>
+      <c r="J156" s="13"/>
+      <c r="K156" s="13"/>
+      <c r="L156" s="13"/>
+      <c r="M156" s="13"/>
+      <c r="N156" s="13"/>
       <c r="P156">
         <f t="shared" si="57"/>
         <v>285.66007977615379</v>
@@ -28492,8 +28491,11 @@
       </c>
     </row>
     <row r="158" spans="2:53" x14ac:dyDescent="0.35">
-      <c r="P158" s="4" t="s">
-        <v>40</v>
+      <c r="Q158" t="s">
+        <v>48</v>
+      </c>
+      <c r="X158" s="14" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="159" spans="2:53" x14ac:dyDescent="0.35">
@@ -28501,7 +28503,7 @@
         <v>15</v>
       </c>
       <c r="C159" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
@@ -28514,11 +28516,15 @@
       <c r="L159" s="1"/>
       <c r="M159" s="1"/>
       <c r="N159" s="1"/>
-      <c r="P159">
+      <c r="Q159">
+        <f>AVERAGE(P136:AA156)</f>
+        <v>179.90467909541755</v>
+      </c>
+      <c r="X159">
         <f>(SUM(AC136:AN154,AC155:AJ155,AC156:AH156)/SUM(AP136:BA154,AP155:AW155,AP156:AU156))^0.5</f>
         <v>286.24477432036861</v>
       </c>
-      <c r="S159" t="s">
+      <c r="AA159" t="s">
         <v>23</v>
       </c>
     </row>
@@ -29404,7 +29410,7 @@
     </row>
     <row r="184" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="185" spans="2:14" x14ac:dyDescent="0.35">
@@ -30457,7 +30463,7 @@
         <v>1</v>
       </c>
       <c r="C205" s="12">
-        <f t="shared" ref="C205:N205" si="100">C155/$C$156</f>
+        <f t="shared" ref="C205:J205" si="100">C155/$C$156</f>
         <v>1.22545205025047</v>
       </c>
       <c r="D205" s="12">
@@ -30498,7 +30504,7 @@
         <v>0</v>
       </c>
       <c r="C206" s="12">
-        <f t="shared" ref="C206:N206" si="101">C156/$C$156</f>
+        <f t="shared" ref="C206:H206" si="101">C156/$C$156</f>
         <v>1</v>
       </c>
       <c r="D206" s="12">

</xml_diff>